<commit_message>
component possible when importing landscape close #70
</commit_message>
<xml_diff>
--- a/src/test/resources/junit/01-import-applications.xlsx
+++ b/src/test/resources/junit/01-import-applications.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Application" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Missing app" sheetId="2" state="hidden" r:id="rId3"/>
+    <sheet name="Component" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="56">
   <si>
     <t xml:space="preserve">application.id</t>
   </si>
@@ -177,6 +178,18 @@
   </si>
   <si>
     <t xml:space="preserve">goAML</t>
+  </si>
+  <si>
+    <t xml:space="preserve">component.id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">component.name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUB.0000001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">COMPONENT-0001-0001</t>
   </si>
 </sst>
 </file>
@@ -380,13 +393,13 @@
   </sheetPr>
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="C2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.85"/>
@@ -557,7 +570,7 @@
       <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="35.12"/>
   </cols>
@@ -689,6 +702,57 @@
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="26.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.99"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>

</xml_diff>